<commit_message>
Testing alternative approaches to access urbanization distribution
</commit_message>
<xml_diff>
--- a/Data/Test_product_categories.xlsx
+++ b/Data/Test_product_categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/bertiner_ntnu_no/Documents/2_Env_Eng/IOA_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="553" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E31E7F51-6CF5-4CFE-B850-D7F467394402}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E6FF379-42EB-46DD-AC99-F18FD5B7174F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
     <t>Financial intermediation services, insurances</t>
   </si>
   <si>
-    <t>Products of vegetable oils and fats</t>
+    <t>products of Vegetable oils and fats</t>
   </si>
   <si>
     <t>Transmission and distribution of electricity</t>
@@ -302,7 +302,7 @@
     <t>Nuclear fuel</t>
   </si>
   <si>
-    <t>Coke and tar</t>
+    <t>Coke and Tar</t>
   </si>
   <si>
     <t>Sale, maintenance, repair of motor vehicles, motor vehicles parts, motorcycles, motor cycles parts and accessoiries, fuel stations</t>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2B5A38-EE05-4B87-B85E-53A18DBAFCC6}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="I11" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>